<commit_message>
metadata on restoration database
</commit_message>
<xml_diff>
--- a/data/input/Shyamsundaretal.xlsx
+++ b/data/input/Shyamsundaretal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\FOLUR-Restoration-maps\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide Cozza\Documents\GitHub\FOLUR-Restoration-maps\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DAC7B7-F55A-47D2-9914-8302C31F717B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A136A7B2-EEAA-4C92-89DF-2F13057B2570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3BB540F2-8CCF-4901-8099-C5C2E175DEB9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3BB540F2-8CCF-4901-8099-C5C2E175DEB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Shyamsundar et al 2022" sheetId="1" r:id="rId1"/>
@@ -323,20 +323,26 @@
     <t>source</t>
   </si>
   <si>
-    <t>Shyamsundaretal</t>
-  </si>
-  <si>
     <t>Restoration_Potential</t>
+  </si>
+  <si>
+    <t>Shyamsundaretal_2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -701,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D627E3F-55B7-41ED-A223-03866118DC3F}">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B88"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -749,7 +755,7 @@
         <v>92</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -757,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3">
         <v>30523900</v>
@@ -769,7 +775,7 @@
         <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -777,7 +783,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4">
         <v>2600</v>
@@ -789,7 +795,7 @@
         <v>92</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -797,7 +803,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5">
         <v>4000</v>
@@ -809,7 +815,7 @@
         <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -817,7 +823,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -829,7 +835,7 @@
         <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -837,7 +843,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7">
         <v>502800</v>
@@ -849,7 +855,7 @@
         <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -857,7 +863,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8">
         <v>16600</v>
@@ -869,7 +875,7 @@
         <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -877,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9">
         <v>1170400</v>
@@ -889,7 +895,7 @@
         <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -897,7 +903,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10">
         <v>84325300</v>
@@ -909,7 +915,7 @@
         <v>92</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -917,7 +923,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11">
         <v>65300</v>
@@ -929,7 +935,7 @@
         <v>92</v>
       </c>
       <c r="F11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -937,7 +943,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -949,7 +955,7 @@
         <v>92</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -957,7 +963,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13">
         <v>204500</v>
@@ -969,7 +975,7 @@
         <v>92</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -977,7 +983,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14">
         <v>4443000</v>
@@ -989,7 +995,7 @@
         <v>92</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -997,7 +1003,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15">
         <v>10793400</v>
@@ -1009,7 +1015,7 @@
         <v>92</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1017,7 +1023,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16">
         <v>14753100</v>
@@ -1029,7 +1035,7 @@
         <v>92</v>
       </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1037,7 +1043,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17">
         <v>54700</v>
@@ -1049,7 +1055,7 @@
         <v>92</v>
       </c>
       <c r="F17" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1057,7 +1063,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18">
         <v>10504100</v>
@@ -1069,7 +1075,7 @@
         <v>92</v>
       </c>
       <c r="F18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1077,7 +1083,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19">
         <v>22188800</v>
@@ -1089,7 +1095,7 @@
         <v>92</v>
       </c>
       <c r="F19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1097,7 +1103,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20">
         <v>34800</v>
@@ -1109,7 +1115,7 @@
         <v>92</v>
       </c>
       <c r="F20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1117,7 +1123,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21">
         <v>7660400</v>
@@ -1129,7 +1135,7 @@
         <v>92</v>
       </c>
       <c r="F21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1137,7 +1143,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22">
         <v>2492500</v>
@@ -1149,7 +1155,7 @@
         <v>92</v>
       </c>
       <c r="F22" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1157,7 +1163,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23">
         <v>13049600</v>
@@ -1169,7 +1175,7 @@
         <v>92</v>
       </c>
       <c r="F23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1177,7 +1183,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24">
         <v>2371600</v>
@@ -1189,7 +1195,7 @@
         <v>92</v>
       </c>
       <c r="F24" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1197,7 +1203,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25">
         <v>80999700</v>
@@ -1209,7 +1215,7 @@
         <v>92</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1217,7 +1223,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1229,7 +1235,7 @@
         <v>92</v>
       </c>
       <c r="F26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1237,7 +1243,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27">
         <v>600</v>
@@ -1249,7 +1255,7 @@
         <v>92</v>
       </c>
       <c r="F27" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1257,7 +1263,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28">
         <v>1926200</v>
@@ -1269,7 +1275,7 @@
         <v>92</v>
       </c>
       <c r="F28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1277,7 +1283,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29">
         <v>5715400</v>
@@ -1289,7 +1295,7 @@
         <v>92</v>
       </c>
       <c r="F29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1297,7 +1303,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30">
         <v>588400</v>
@@ -1309,7 +1315,7 @@
         <v>92</v>
       </c>
       <c r="F30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1317,7 +1323,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31">
         <v>6966300</v>
@@ -1329,7 +1335,7 @@
         <v>92</v>
       </c>
       <c r="F31" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1337,7 +1343,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C32">
         <v>28100</v>
@@ -1349,7 +1355,7 @@
         <v>92</v>
       </c>
       <c r="F32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1357,7 +1363,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C33">
         <v>20700</v>
@@ -1369,7 +1375,7 @@
         <v>92</v>
       </c>
       <c r="F33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1377,7 +1383,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C34">
         <v>202400</v>
@@ -1389,7 +1395,7 @@
         <v>92</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1397,7 +1403,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C35">
         <v>2204500</v>
@@ -1409,7 +1415,7 @@
         <v>92</v>
       </c>
       <c r="F35" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1417,7 +1423,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36">
         <v>5330400</v>
@@ -1429,7 +1435,7 @@
         <v>92</v>
       </c>
       <c r="F36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1437,7 +1443,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C37">
         <v>3200</v>
@@ -1449,7 +1455,7 @@
         <v>92</v>
       </c>
       <c r="F37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1457,7 +1463,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C38">
         <v>18300</v>
@@ -1469,7 +1475,7 @@
         <v>92</v>
       </c>
       <c r="F38" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1477,7 +1483,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39">
         <v>4118100</v>
@@ -1489,7 +1495,7 @@
         <v>92</v>
       </c>
       <c r="F39" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1497,7 +1503,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40">
         <v>4744900</v>
@@ -1509,7 +1515,7 @@
         <v>92</v>
       </c>
       <c r="F40" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1517,7 +1523,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C41">
         <v>648800</v>
@@ -1529,7 +1535,7 @@
         <v>92</v>
       </c>
       <c r="F41" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1537,7 +1543,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42">
         <v>579300</v>
@@ -1549,7 +1555,7 @@
         <v>92</v>
       </c>
       <c r="F42" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1557,7 +1563,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43">
         <v>4009800</v>
@@ -1569,7 +1575,7 @@
         <v>92</v>
       </c>
       <c r="F43" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1577,7 +1583,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44">
         <v>9443400</v>
@@ -1589,7 +1595,7 @@
         <v>92</v>
       </c>
       <c r="F44" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1597,7 +1603,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C45">
         <v>42330800</v>
@@ -1609,7 +1615,7 @@
         <v>92</v>
       </c>
       <c r="F45" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1617,7 +1623,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46">
         <v>419500</v>
@@ -1629,7 +1635,7 @@
         <v>92</v>
       </c>
       <c r="F46" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1637,7 +1643,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C47">
         <v>1769600</v>
@@ -1649,7 +1655,7 @@
         <v>92</v>
       </c>
       <c r="F47" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1657,7 +1663,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C48">
         <v>5455400</v>
@@ -1669,7 +1675,7 @@
         <v>92</v>
       </c>
       <c r="F48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1677,7 +1683,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C49">
         <v>1427000</v>
@@ -1689,7 +1695,7 @@
         <v>92</v>
       </c>
       <c r="F49" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1697,7 +1703,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C50">
         <v>1969400</v>
@@ -1709,7 +1715,7 @@
         <v>92</v>
       </c>
       <c r="F50" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1717,7 +1723,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C51">
         <v>8533600</v>
@@ -1729,7 +1735,7 @@
         <v>92</v>
       </c>
       <c r="F51" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1737,7 +1743,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C52">
         <v>751300</v>
@@ -1749,7 +1755,7 @@
         <v>92</v>
       </c>
       <c r="F52" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1757,7 +1763,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C53">
         <v>33900</v>
@@ -1769,7 +1775,7 @@
         <v>92</v>
       </c>
       <c r="F53" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1777,7 +1783,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C54">
         <v>4900</v>
@@ -1789,7 +1795,7 @@
         <v>92</v>
       </c>
       <c r="F54" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1797,7 +1803,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C55">
         <v>20051900</v>
@@ -1809,7 +1815,7 @@
         <v>92</v>
       </c>
       <c r="F55" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1817,7 +1823,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C56">
         <v>300</v>
@@ -1829,7 +1835,7 @@
         <v>92</v>
       </c>
       <c r="F56" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1837,7 +1843,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C57">
         <v>200</v>
@@ -1849,7 +1855,7 @@
         <v>92</v>
       </c>
       <c r="F57" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1857,7 +1863,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C58">
         <v>10657100</v>
@@ -1869,7 +1875,7 @@
         <v>92</v>
       </c>
       <c r="F58" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1877,7 +1883,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C59">
         <v>12462000</v>
@@ -1889,7 +1895,7 @@
         <v>92</v>
       </c>
       <c r="F59" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1897,7 +1903,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C60">
         <v>5596400</v>
@@ -1909,7 +1915,7 @@
         <v>92</v>
       </c>
       <c r="F60" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1917,7 +1923,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C61">
         <v>5806600</v>
@@ -1929,7 +1935,7 @@
         <v>92</v>
       </c>
       <c r="F61" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1937,7 +1943,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C62">
         <v>2899500</v>
@@ -1949,7 +1955,7 @@
         <v>92</v>
       </c>
       <c r="F62" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1957,7 +1963,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C63">
         <v>3999100</v>
@@ -1969,7 +1975,7 @@
         <v>92</v>
       </c>
       <c r="F63" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1977,7 +1983,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C64">
         <v>2990800</v>
@@ -1989,7 +1995,7 @@
         <v>92</v>
       </c>
       <c r="F64" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1997,7 +2003,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C65">
         <v>10486100</v>
@@ -2009,7 +2015,7 @@
         <v>92</v>
       </c>
       <c r="F65" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -2017,7 +2023,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C66">
         <v>307000</v>
@@ -2029,7 +2035,7 @@
         <v>92</v>
       </c>
       <c r="F66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2037,7 +2043,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C67">
         <v>95300</v>
@@ -2049,7 +2055,7 @@
         <v>92</v>
       </c>
       <c r="F67" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2057,7 +2063,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C68">
         <v>4000</v>
@@ -2069,7 +2075,7 @@
         <v>92</v>
       </c>
       <c r="F68" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2077,7 +2083,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C69">
         <v>4500</v>
@@ -2089,7 +2095,7 @@
         <v>92</v>
       </c>
       <c r="F69" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2097,7 +2103,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C70">
         <v>5600</v>
@@ -2109,7 +2115,7 @@
         <v>92</v>
       </c>
       <c r="F70" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2117,7 +2123,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C71">
         <v>4900</v>
@@ -2129,7 +2135,7 @@
         <v>92</v>
       </c>
       <c r="F71" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2137,7 +2143,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C72">
         <v>3186300</v>
@@ -2149,7 +2155,7 @@
         <v>92</v>
       </c>
       <c r="F72" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2157,7 +2163,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C73">
         <v>28100</v>
@@ -2169,7 +2175,7 @@
         <v>92</v>
       </c>
       <c r="F73" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2177,7 +2183,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C74">
         <v>2155600</v>
@@ -2189,7 +2195,7 @@
         <v>92</v>
       </c>
       <c r="F74" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2197,7 +2203,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C75">
         <v>2352600</v>
@@ -2209,7 +2215,7 @@
         <v>92</v>
       </c>
       <c r="F75" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2217,7 +2223,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C76">
         <v>89600</v>
@@ -2229,7 +2235,7 @@
         <v>92</v>
       </c>
       <c r="F76" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2237,7 +2243,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C77">
         <v>21629000</v>
@@ -2249,7 +2255,7 @@
         <v>92</v>
       </c>
       <c r="F77" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2257,7 +2263,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C78">
         <v>11540400</v>
@@ -2269,7 +2275,7 @@
         <v>92</v>
       </c>
       <c r="F78" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2277,7 +2283,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C79">
         <v>324000</v>
@@ -2289,7 +2295,7 @@
         <v>92</v>
       </c>
       <c r="F79" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2297,7 +2303,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C80">
         <v>498600</v>
@@ -2309,7 +2315,7 @@
         <v>92</v>
       </c>
       <c r="F80" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2317,7 +2323,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C81">
         <v>88200</v>
@@ -2329,7 +2335,7 @@
         <v>92</v>
       </c>
       <c r="F81" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2337,7 +2343,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C82">
         <v>4847800</v>
@@ -2349,7 +2355,7 @@
         <v>92</v>
       </c>
       <c r="F82" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2357,7 +2363,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C83">
         <v>1300</v>
@@ -2369,7 +2375,7 @@
         <v>92</v>
       </c>
       <c r="F83" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2377,7 +2383,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C84">
         <v>11618600</v>
@@ -2389,7 +2395,7 @@
         <v>92</v>
       </c>
       <c r="F84" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2397,7 +2403,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C85">
         <v>8520600</v>
@@ -2409,7 +2415,7 @@
         <v>92</v>
       </c>
       <c r="F85" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -2417,7 +2423,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C86">
         <v>500</v>
@@ -2429,7 +2435,7 @@
         <v>92</v>
       </c>
       <c r="F86" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -2437,7 +2443,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2449,7 +2455,7 @@
         <v>92</v>
       </c>
       <c r="F87" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -2457,7 +2463,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C88">
         <v>8283400</v>
@@ -2469,10 +2475,11 @@
         <v>92</v>
       </c>
       <c r="F88" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>